<commit_message>
Update ReadMe file & add the requirements file
</commit_message>
<xml_diff>
--- a/output/beneficial.xlsx
+++ b/output/beneficial.xlsx
@@ -519,14 +519,14 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Haemophilus</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D4" t="n">
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0.005704838249311408</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="5">
@@ -542,14 +542,14 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Neisseria</t>
+          <t>Haemophilus</t>
         </is>
       </c>
       <c r="D5" t="n">
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>0.0003247717504744928</v>
+        <v>0.005704838249311408</v>
       </c>
     </row>
     <row r="6">
@@ -565,14 +565,14 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Neisseria</t>
         </is>
       </c>
       <c r="D6" t="n">
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.0003247717504744928</v>
       </c>
     </row>
     <row r="7">
@@ -611,14 +611,14 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Ezakiella</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D8" t="n">
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>0.002980975725860719</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="9">
@@ -634,14 +634,14 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Varibaculum</t>
         </is>
       </c>
       <c r="D9" t="n">
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.006990870234154651</v>
       </c>
     </row>
     <row r="10">
@@ -657,14 +657,14 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Varibaculum</t>
+          <t>Ezakiella</t>
         </is>
       </c>
       <c r="D10" t="n">
         <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>0.006990870234154651</v>
+        <v>0.002980975725860719</v>
       </c>
     </row>
     <row r="11">
@@ -795,14 +795,14 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Haemophilus</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D16" t="n">
         <v>0</v>
       </c>
       <c r="E16" t="n">
-        <v>0.005704838249311408</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="17">
@@ -818,14 +818,14 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Neisseria</t>
+          <t>Haemophilus</t>
         </is>
       </c>
       <c r="D17" t="n">
         <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>0.0003247717504744928</v>
+        <v>0.005704838249311408</v>
       </c>
     </row>
     <row r="18">
@@ -841,14 +841,14 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Neisseria</t>
         </is>
       </c>
       <c r="D18" t="n">
         <v>0</v>
       </c>
       <c r="E18" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.0003247717504744928</v>
       </c>
     </row>
     <row r="19">
@@ -887,14 +887,14 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Ezakiella</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D20" t="n">
         <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>0.002980975725860719</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="21">
@@ -910,14 +910,14 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Varibaculum</t>
         </is>
       </c>
       <c r="D21" t="n">
         <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.006990870234154651</v>
       </c>
     </row>
     <row r="22">
@@ -933,14 +933,14 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Varibaculum</t>
+          <t>Ezakiella</t>
         </is>
       </c>
       <c r="D22" t="n">
         <v>0</v>
       </c>
       <c r="E22" t="n">
-        <v>0.006990870234154651</v>
+        <v>0.002980975725860719</v>
       </c>
     </row>
     <row r="23">
@@ -1370,14 +1370,14 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Neisseria</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D41" t="n">
         <v>0</v>
       </c>
       <c r="E41" t="n">
-        <v>0.0003247717504744928</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="42">
@@ -1393,14 +1393,14 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Neisseria</t>
         </is>
       </c>
       <c r="D42" t="n">
         <v>0</v>
       </c>
       <c r="E42" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.0003247717504744928</v>
       </c>
     </row>
     <row r="43">
@@ -1462,14 +1462,14 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Ezakiella</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D45" t="n">
         <v>0</v>
       </c>
       <c r="E45" t="n">
-        <v>0.002980975725860719</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="46">
@@ -1485,14 +1485,14 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Ezakiella</t>
         </is>
       </c>
       <c r="D46" t="n">
         <v>0</v>
       </c>
       <c r="E46" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.002980975725860719</v>
       </c>
     </row>
     <row r="47">
@@ -1692,14 +1692,14 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Prevotella</t>
         </is>
       </c>
       <c r="D55" t="n">
         <v>7.05641604629009e-05</v>
       </c>
       <c r="E55" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.05315508228653677</v>
       </c>
     </row>
     <row r="56">
@@ -1715,14 +1715,14 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Prevotella</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D56" t="n">
         <v>7.05641604629009e-05</v>
       </c>
       <c r="E56" t="n">
-        <v>0.05315508228653677</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="57">
@@ -1738,14 +1738,14 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Ezakiella</t>
+          <t>Varibaculum</t>
         </is>
       </c>
       <c r="D57" t="n">
         <v>0</v>
       </c>
       <c r="E57" t="n">
-        <v>0.002980975725860719</v>
+        <v>0.006990870234154651</v>
       </c>
     </row>
     <row r="58">
@@ -1761,14 +1761,14 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Varibaculum</t>
+          <t>Ezakiella</t>
         </is>
       </c>
       <c r="D58" t="n">
         <v>0</v>
       </c>
       <c r="E58" t="n">
-        <v>0.006990870234154651</v>
+        <v>0.002980975725860719</v>
       </c>
     </row>
     <row r="59">
@@ -1899,14 +1899,14 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Haemophilus</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D64" t="n">
         <v>0</v>
       </c>
       <c r="E64" t="n">
-        <v>0.005704838249311408</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="65">
@@ -1922,14 +1922,14 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Neisseria</t>
+          <t>Haemophilus</t>
         </is>
       </c>
       <c r="D65" t="n">
         <v>0</v>
       </c>
       <c r="E65" t="n">
-        <v>0.0003247717504744928</v>
+        <v>0.005704838249311408</v>
       </c>
     </row>
     <row r="66">
@@ -1945,14 +1945,14 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Neisseria</t>
         </is>
       </c>
       <c r="D66" t="n">
         <v>0</v>
       </c>
       <c r="E66" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.0003247717504744928</v>
       </c>
     </row>
     <row r="67">
@@ -1991,14 +1991,14 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Ezakiella</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D68" t="n">
         <v>0</v>
       </c>
       <c r="E68" t="n">
-        <v>0.002980975725860719</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="69">
@@ -2014,14 +2014,14 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Varibaculum</t>
         </is>
       </c>
       <c r="D69" t="n">
         <v>0</v>
       </c>
       <c r="E69" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.006990870234154651</v>
       </c>
     </row>
     <row r="70">
@@ -2037,14 +2037,14 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Varibaculum</t>
+          <t>Ezakiella</t>
         </is>
       </c>
       <c r="D70" t="n">
         <v>0</v>
       </c>
       <c r="E70" t="n">
-        <v>0.006990870234154651</v>
+        <v>0.002980975725860719</v>
       </c>
     </row>
     <row r="71">
@@ -2474,14 +2474,14 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Neisseria</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D89" t="n">
         <v>0</v>
       </c>
       <c r="E89" t="n">
-        <v>0.0003247717504744928</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="90">
@@ -2497,14 +2497,14 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Neisseria</t>
         </is>
       </c>
       <c r="D90" t="n">
         <v>0</v>
       </c>
       <c r="E90" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.0003247717504744928</v>
       </c>
     </row>
     <row r="91">
@@ -2543,14 +2543,14 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Ezakiella</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D92" t="n">
         <v>0</v>
       </c>
       <c r="E92" t="n">
-        <v>0.002980975725860719</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="93">
@@ -2566,14 +2566,14 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Varibaculum</t>
         </is>
       </c>
       <c r="D93" t="n">
         <v>0</v>
       </c>
       <c r="E93" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.006990870234154651</v>
       </c>
     </row>
     <row r="94">
@@ -2589,14 +2589,14 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>Varibaculum</t>
+          <t>Ezakiella</t>
         </is>
       </c>
       <c r="D94" t="n">
         <v>0</v>
       </c>
       <c r="E94" t="n">
-        <v>0.006990870234154651</v>
+        <v>0.002980975725860719</v>
       </c>
     </row>
     <row r="95">
@@ -2750,14 +2750,14 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>Neisseria</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D101" t="n">
         <v>0</v>
       </c>
       <c r="E101" t="n">
-        <v>0.0003247717504744928</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="102">
@@ -2773,14 +2773,14 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Neisseria</t>
         </is>
       </c>
       <c r="D102" t="n">
         <v>0</v>
       </c>
       <c r="E102" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.0003247717504744928</v>
       </c>
     </row>
     <row r="103">
@@ -2842,14 +2842,14 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>Ezakiella</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D105" t="n">
         <v>0</v>
       </c>
       <c r="E105" t="n">
-        <v>0.002980975725860719</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="106">
@@ -2865,14 +2865,14 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Ezakiella</t>
         </is>
       </c>
       <c r="D106" t="n">
         <v>0</v>
       </c>
       <c r="E106" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.002980975725860719</v>
       </c>
     </row>
     <row r="107">
@@ -3118,14 +3118,14 @@
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>Ezakiella</t>
+          <t>Varibaculum</t>
         </is>
       </c>
       <c r="D117" t="n">
         <v>0</v>
       </c>
       <c r="E117" t="n">
-        <v>0.002980975725860719</v>
+        <v>0.006990870234154651</v>
       </c>
     </row>
     <row r="118">
@@ -3141,14 +3141,14 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>Varibaculum</t>
+          <t>Ezakiella</t>
         </is>
       </c>
       <c r="D118" t="n">
         <v>0</v>
       </c>
       <c r="E118" t="n">
-        <v>0.006990870234154651</v>
+        <v>0.002980975725860719</v>
       </c>
     </row>
     <row r="119">
@@ -3279,14 +3279,14 @@
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>Haemophilus</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D124" t="n">
         <v>0</v>
       </c>
       <c r="E124" t="n">
-        <v>0.005704838249311408</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="125">
@@ -3302,14 +3302,14 @@
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>Neisseria</t>
+          <t>Haemophilus</t>
         </is>
       </c>
       <c r="D125" t="n">
         <v>0</v>
       </c>
       <c r="E125" t="n">
-        <v>0.0003247717504744928</v>
+        <v>0.005704838249311408</v>
       </c>
     </row>
     <row r="126">
@@ -3325,14 +3325,14 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Neisseria</t>
         </is>
       </c>
       <c r="D126" t="n">
         <v>0</v>
       </c>
       <c r="E126" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.0003247717504744928</v>
       </c>
     </row>
     <row r="127">
@@ -4406,14 +4406,14 @@
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>Neisseria</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D173" t="n">
         <v>0</v>
       </c>
       <c r="E173" t="n">
-        <v>0.0003247717504744928</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="174">
@@ -4429,14 +4429,14 @@
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Neisseria</t>
         </is>
       </c>
       <c r="D174" t="n">
         <v>0</v>
       </c>
       <c r="E174" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.0003247717504744928</v>
       </c>
     </row>
     <row r="175">
@@ -5510,14 +5510,14 @@
       </c>
       <c r="C221" t="inlineStr">
         <is>
-          <t>Neisseria</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D221" t="n">
         <v>0</v>
       </c>
       <c r="E221" t="n">
-        <v>0.0003247717504744928</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="222">
@@ -5533,14 +5533,14 @@
       </c>
       <c r="C222" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Neisseria</t>
         </is>
       </c>
       <c r="D222" t="n">
         <v>0</v>
       </c>
       <c r="E222" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.0003247717504744928</v>
       </c>
     </row>
     <row r="223">
@@ -5602,14 +5602,14 @@
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>Ezakiella</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D225" t="n">
         <v>0</v>
       </c>
       <c r="E225" t="n">
-        <v>0.002980975725860719</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="226">
@@ -5625,14 +5625,14 @@
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Ezakiella</t>
         </is>
       </c>
       <c r="D226" t="n">
         <v>0</v>
       </c>
       <c r="E226" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.002980975725860719</v>
       </c>
     </row>
     <row r="227">
@@ -6062,14 +6062,14 @@
       </c>
       <c r="C245" t="inlineStr">
         <is>
-          <t>Neisseria</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D245" t="n">
         <v>0</v>
       </c>
       <c r="E245" t="n">
-        <v>0.0003247717504744928</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="246">
@@ -6085,14 +6085,14 @@
       </c>
       <c r="C246" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Neisseria</t>
         </is>
       </c>
       <c r="D246" t="n">
         <v>0</v>
       </c>
       <c r="E246" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.0003247717504744928</v>
       </c>
     </row>
     <row r="247">
@@ -6131,14 +6131,14 @@
       </c>
       <c r="C248" t="inlineStr">
         <is>
-          <t>Ezakiella</t>
+          <t>Varibaculum</t>
         </is>
       </c>
       <c r="D248" t="n">
         <v>5.945303210463734e-05</v>
       </c>
       <c r="E248" t="n">
-        <v>0.002980975725860719</v>
+        <v>0.006990870234154651</v>
       </c>
     </row>
     <row r="249">
@@ -6154,14 +6154,14 @@
       </c>
       <c r="C249" t="inlineStr">
         <is>
-          <t>Varibaculum</t>
+          <t>Ezakiella</t>
         </is>
       </c>
       <c r="D249" t="n">
         <v>5.945303210463734e-05</v>
       </c>
       <c r="E249" t="n">
-        <v>0.006990870234154651</v>
+        <v>0.002980975725860719</v>
       </c>
     </row>
     <row r="250">
@@ -6867,14 +6867,14 @@
       </c>
       <c r="C280" t="inlineStr">
         <is>
-          <t>Haemophilus</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D280" t="n">
         <v>0</v>
       </c>
       <c r="E280" t="n">
-        <v>0.005704838249311408</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="281">
@@ -6890,14 +6890,14 @@
       </c>
       <c r="C281" t="inlineStr">
         <is>
-          <t>Neisseria</t>
+          <t>Haemophilus</t>
         </is>
       </c>
       <c r="D281" t="n">
         <v>0</v>
       </c>
       <c r="E281" t="n">
-        <v>0.0003247717504744928</v>
+        <v>0.005704838249311408</v>
       </c>
     </row>
     <row r="282">
@@ -6913,14 +6913,14 @@
       </c>
       <c r="C282" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Neisseria</t>
         </is>
       </c>
       <c r="D282" t="n">
         <v>0</v>
       </c>
       <c r="E282" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.0003247717504744928</v>
       </c>
     </row>
     <row r="283">
@@ -6982,14 +6982,14 @@
       </c>
       <c r="C285" t="inlineStr">
         <is>
-          <t>Ezakiella</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D285" t="n">
         <v>0</v>
       </c>
       <c r="E285" t="n">
-        <v>0.002980975725860719</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="286">
@@ -7005,14 +7005,14 @@
       </c>
       <c r="C286" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Ezakiella</t>
         </is>
       </c>
       <c r="D286" t="n">
         <v>0</v>
       </c>
       <c r="E286" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.002980975725860719</v>
       </c>
     </row>
     <row r="287">
@@ -7143,14 +7143,14 @@
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>Haemophilus</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D292" t="n">
         <v>0</v>
       </c>
       <c r="E292" t="n">
-        <v>0.005704838249311408</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="293">
@@ -7166,14 +7166,14 @@
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>Neisseria</t>
+          <t>Haemophilus</t>
         </is>
       </c>
       <c r="D293" t="n">
         <v>0</v>
       </c>
       <c r="E293" t="n">
-        <v>0.0003247717504744928</v>
+        <v>0.005704838249311408</v>
       </c>
     </row>
     <row r="294">
@@ -7189,14 +7189,14 @@
       </c>
       <c r="C294" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Neisseria</t>
         </is>
       </c>
       <c r="D294" t="n">
         <v>0</v>
       </c>
       <c r="E294" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.0003247717504744928</v>
       </c>
     </row>
     <row r="295">
@@ -7258,14 +7258,14 @@
       </c>
       <c r="C297" t="inlineStr">
         <is>
-          <t>Ezakiella</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D297" t="n">
         <v>0</v>
       </c>
       <c r="E297" t="n">
-        <v>0.002980975725860719</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="298">
@@ -7281,14 +7281,14 @@
       </c>
       <c r="C298" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Ezakiella</t>
         </is>
       </c>
       <c r="D298" t="n">
         <v>0</v>
       </c>
       <c r="E298" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.002980975725860719</v>
       </c>
     </row>
     <row r="299">
@@ -7534,14 +7534,14 @@
       </c>
       <c r="C309" t="inlineStr">
         <is>
-          <t>Ezakiella</t>
+          <t>Varibaculum</t>
         </is>
       </c>
       <c r="D309" t="n">
         <v>0</v>
       </c>
       <c r="E309" t="n">
-        <v>0.002980975725860719</v>
+        <v>0.006990870234154651</v>
       </c>
     </row>
     <row r="310">
@@ -7557,14 +7557,14 @@
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>Varibaculum</t>
+          <t>Ezakiella</t>
         </is>
       </c>
       <c r="D310" t="n">
         <v>0</v>
       </c>
       <c r="E310" t="n">
-        <v>0.006990870234154651</v>
+        <v>0.002980975725860719</v>
       </c>
     </row>
     <row r="311">
@@ -8799,14 +8799,14 @@
       </c>
       <c r="C364" t="inlineStr">
         <is>
-          <t>Haemophilus</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D364" t="n">
         <v>0</v>
       </c>
       <c r="E364" t="n">
-        <v>0.005704838249311408</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="365">
@@ -8822,14 +8822,14 @@
       </c>
       <c r="C365" t="inlineStr">
         <is>
-          <t>Neisseria</t>
+          <t>Haemophilus</t>
         </is>
       </c>
       <c r="D365" t="n">
         <v>0</v>
       </c>
       <c r="E365" t="n">
-        <v>0.0003247717504744928</v>
+        <v>0.005704838249311408</v>
       </c>
     </row>
     <row r="366">
@@ -8845,14 +8845,14 @@
       </c>
       <c r="C366" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Neisseria</t>
         </is>
       </c>
       <c r="D366" t="n">
         <v>0</v>
       </c>
       <c r="E366" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.0003247717504744928</v>
       </c>
     </row>
     <row r="367">
@@ -8914,14 +8914,14 @@
       </c>
       <c r="C369" t="inlineStr">
         <is>
-          <t>Ezakiella</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D369" t="n">
         <v>0</v>
       </c>
       <c r="E369" t="n">
-        <v>0.002980975725860719</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="370">
@@ -8937,14 +8937,14 @@
       </c>
       <c r="C370" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Ezakiella</t>
         </is>
       </c>
       <c r="D370" t="n">
         <v>0</v>
       </c>
       <c r="E370" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.002980975725860719</v>
       </c>
     </row>
     <row r="371">
@@ -9098,14 +9098,14 @@
       </c>
       <c r="C377" t="inlineStr">
         <is>
-          <t>Neisseria</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D377" t="n">
         <v>0</v>
       </c>
       <c r="E377" t="n">
-        <v>0.0003247717504744928</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="378">
@@ -9121,14 +9121,14 @@
       </c>
       <c r="C378" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Neisseria</t>
         </is>
       </c>
       <c r="D378" t="n">
         <v>0</v>
       </c>
       <c r="E378" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.0003247717504744928</v>
       </c>
     </row>
     <row r="379">
@@ -9351,14 +9351,14 @@
       </c>
       <c r="C388" t="inlineStr">
         <is>
-          <t>Haemophilus</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D388" t="n">
         <v>0</v>
       </c>
       <c r="E388" t="n">
-        <v>0.005704838249311408</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="389">
@@ -9374,14 +9374,14 @@
       </c>
       <c r="C389" t="inlineStr">
         <is>
-          <t>Neisseria</t>
+          <t>Haemophilus</t>
         </is>
       </c>
       <c r="D389" t="n">
         <v>0</v>
       </c>
       <c r="E389" t="n">
-        <v>0.0003247717504744928</v>
+        <v>0.005704838249311408</v>
       </c>
     </row>
     <row r="390">
@@ -9397,14 +9397,14 @@
       </c>
       <c r="C390" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Neisseria</t>
         </is>
       </c>
       <c r="D390" t="n">
         <v>0</v>
       </c>
       <c r="E390" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.0003247717504744928</v>
       </c>
     </row>
     <row r="391">
@@ -9466,14 +9466,14 @@
       </c>
       <c r="C393" t="inlineStr">
         <is>
-          <t>Ezakiella</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D393" t="n">
         <v>0</v>
       </c>
       <c r="E393" t="n">
-        <v>0.002980975725860719</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="394">
@@ -9489,14 +9489,14 @@
       </c>
       <c r="C394" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Ezakiella</t>
         </is>
       </c>
       <c r="D394" t="n">
         <v>0</v>
       </c>
       <c r="E394" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.002980975725860719</v>
       </c>
     </row>
     <row r="395">
@@ -9926,14 +9926,14 @@
       </c>
       <c r="C413" t="inlineStr">
         <is>
-          <t>Neisseria</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D413" t="n">
         <v>0</v>
       </c>
       <c r="E413" t="n">
-        <v>0.0003247717504744928</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="414">
@@ -9949,14 +9949,14 @@
       </c>
       <c r="C414" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Neisseria</t>
         </is>
       </c>
       <c r="D414" t="n">
         <v>0</v>
       </c>
       <c r="E414" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.0003247717504744928</v>
       </c>
     </row>
     <row r="415">
@@ -10294,14 +10294,14 @@
       </c>
       <c r="C429" t="inlineStr">
         <is>
-          <t>Ezakiella</t>
+          <t>Varibaculum</t>
         </is>
       </c>
       <c r="D429" t="n">
         <v>4.650297619047619e-05</v>
       </c>
       <c r="E429" t="n">
-        <v>0.002980975725860719</v>
+        <v>0.006990870234154651</v>
       </c>
     </row>
     <row r="430">
@@ -10317,14 +10317,14 @@
       </c>
       <c r="C430" t="inlineStr">
         <is>
-          <t>Varibaculum</t>
+          <t>Ezakiella</t>
         </is>
       </c>
       <c r="D430" t="n">
         <v>4.650297619047619e-05</v>
       </c>
       <c r="E430" t="n">
-        <v>0.006990870234154651</v>
+        <v>0.002980975725860719</v>
       </c>
     </row>
     <row r="431">
@@ -10731,14 +10731,14 @@
       </c>
       <c r="C448" t="inlineStr">
         <is>
-          <t>Haemophilus</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D448" t="n">
         <v>6.912283127116886e-05</v>
       </c>
       <c r="E448" t="n">
-        <v>0.005704838249311408</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="449">
@@ -10754,14 +10754,14 @@
       </c>
       <c r="C449" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Haemophilus</t>
         </is>
       </c>
       <c r="D449" t="n">
         <v>6.912283127116886e-05</v>
       </c>
       <c r="E449" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.005704838249311408</v>
       </c>
     </row>
     <row r="450">
@@ -10823,14 +10823,14 @@
       </c>
       <c r="C452" t="inlineStr">
         <is>
-          <t>Ezakiella</t>
+          <t>Varibaculum</t>
         </is>
       </c>
       <c r="D452" t="n">
         <v>0.0001382456625423</v>
       </c>
       <c r="E452" t="n">
-        <v>0.002980975725860719</v>
+        <v>0.006990870234154651</v>
       </c>
     </row>
     <row r="453">
@@ -10846,14 +10846,14 @@
       </c>
       <c r="C453" t="inlineStr">
         <is>
-          <t>Varibaculum</t>
+          <t>Ezakiella</t>
         </is>
       </c>
       <c r="D453" t="n">
         <v>0.0001382456625423</v>
       </c>
       <c r="E453" t="n">
-        <v>0.006990870234154651</v>
+        <v>0.002980975725860719</v>
       </c>
     </row>
     <row r="454">
@@ -11007,14 +11007,14 @@
       </c>
       <c r="C460" t="inlineStr">
         <is>
-          <t>Haemophilus</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D460" t="n">
         <v>4.561627588723656e-05</v>
       </c>
       <c r="E460" t="n">
-        <v>0.005704838249311408</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="461">
@@ -11030,14 +11030,14 @@
       </c>
       <c r="C461" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Haemophilus</t>
         </is>
       </c>
       <c r="D461" t="n">
         <v>4.561627588723656e-05</v>
       </c>
       <c r="E461" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.005704838249311408</v>
       </c>
     </row>
     <row r="462">
@@ -11398,14 +11398,14 @@
       </c>
       <c r="C477" t="inlineStr">
         <is>
-          <t>Ezakiella</t>
+          <t>Varibaculum</t>
         </is>
       </c>
       <c r="D477" t="n">
         <v>0</v>
       </c>
       <c r="E477" t="n">
-        <v>0.002980975725860719</v>
+        <v>0.006990870234154651</v>
       </c>
     </row>
     <row r="478">
@@ -11421,14 +11421,14 @@
       </c>
       <c r="C478" t="inlineStr">
         <is>
-          <t>Varibaculum</t>
+          <t>Ezakiella</t>
         </is>
       </c>
       <c r="D478" t="n">
         <v>0</v>
       </c>
       <c r="E478" t="n">
-        <v>0.006990870234154651</v>
+        <v>0.002980975725860719</v>
       </c>
     </row>
     <row r="479">
@@ -11858,14 +11858,14 @@
       </c>
       <c r="C497" t="inlineStr">
         <is>
-          <t>Neisseria</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D497" t="n">
         <v>0</v>
       </c>
       <c r="E497" t="n">
-        <v>0.0003247717504744928</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="498">
@@ -11881,14 +11881,14 @@
       </c>
       <c r="C498" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Neisseria</t>
         </is>
       </c>
       <c r="D498" t="n">
         <v>0</v>
       </c>
       <c r="E498" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.0003247717504744928</v>
       </c>
     </row>
     <row r="499">
@@ -11927,14 +11927,14 @@
       </c>
       <c r="C500" t="inlineStr">
         <is>
-          <t>Ezakiella</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D500" t="n">
         <v>0</v>
       </c>
       <c r="E500" t="n">
-        <v>0.002980975725860719</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="501">
@@ -11950,14 +11950,14 @@
       </c>
       <c r="C501" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Varibaculum</t>
         </is>
       </c>
       <c r="D501" t="n">
         <v>0</v>
       </c>
       <c r="E501" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.006990870234154651</v>
       </c>
     </row>
     <row r="502">
@@ -11973,14 +11973,14 @@
       </c>
       <c r="C502" t="inlineStr">
         <is>
-          <t>Varibaculum</t>
+          <t>Ezakiella</t>
         </is>
       </c>
       <c r="D502" t="n">
         <v>0</v>
       </c>
       <c r="E502" t="n">
-        <v>0.006990870234154651</v>
+        <v>0.002980975725860719</v>
       </c>
     </row>
     <row r="503">
@@ -12502,14 +12502,14 @@
       </c>
       <c r="C525" t="inlineStr">
         <is>
-          <t>Ezakiella</t>
+          <t>Varibaculum</t>
         </is>
       </c>
       <c r="D525" t="n">
         <v>0</v>
       </c>
       <c r="E525" t="n">
-        <v>0.002980975725860719</v>
+        <v>0.006990870234154651</v>
       </c>
     </row>
     <row r="526">
@@ -12525,14 +12525,14 @@
       </c>
       <c r="C526" t="inlineStr">
         <is>
-          <t>Varibaculum</t>
+          <t>Ezakiella</t>
         </is>
       </c>
       <c r="D526" t="n">
         <v>0</v>
       </c>
       <c r="E526" t="n">
-        <v>0.006990870234154651</v>
+        <v>0.002980975725860719</v>
       </c>
     </row>
     <row r="527">
@@ -12686,14 +12686,14 @@
       </c>
       <c r="C533" t="inlineStr">
         <is>
-          <t>Neisseria</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D533" t="n">
         <v>0</v>
       </c>
       <c r="E533" t="n">
-        <v>0.0003247717504744928</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="534">
@@ -12709,14 +12709,14 @@
       </c>
       <c r="C534" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Neisseria</t>
         </is>
       </c>
       <c r="D534" t="n">
         <v>0</v>
       </c>
       <c r="E534" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.0003247717504744928</v>
       </c>
     </row>
     <row r="535">
@@ -12755,14 +12755,14 @@
       </c>
       <c r="C536" t="inlineStr">
         <is>
-          <t>Ezakiella</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D536" t="n">
         <v>0</v>
       </c>
       <c r="E536" t="n">
-        <v>0.002980975725860719</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="537">
@@ -12778,14 +12778,14 @@
       </c>
       <c r="C537" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Varibaculum</t>
         </is>
       </c>
       <c r="D537" t="n">
         <v>0</v>
       </c>
       <c r="E537" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.006990870234154651</v>
       </c>
     </row>
     <row r="538">
@@ -12801,14 +12801,14 @@
       </c>
       <c r="C538" t="inlineStr">
         <is>
-          <t>Varibaculum</t>
+          <t>Ezakiella</t>
         </is>
       </c>
       <c r="D538" t="n">
         <v>0</v>
       </c>
       <c r="E538" t="n">
-        <v>0.006990870234154651</v>
+        <v>0.002980975725860719</v>
       </c>
     </row>
     <row r="539">
@@ -12939,14 +12939,14 @@
       </c>
       <c r="C544" t="inlineStr">
         <is>
-          <t>Haemophilus</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D544" t="n">
         <v>0</v>
       </c>
       <c r="E544" t="n">
-        <v>0.005704838249311408</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="545">
@@ -12962,14 +12962,14 @@
       </c>
       <c r="C545" t="inlineStr">
         <is>
-          <t>Neisseria</t>
+          <t>Haemophilus</t>
         </is>
       </c>
       <c r="D545" t="n">
         <v>0</v>
       </c>
       <c r="E545" t="n">
-        <v>0.0003247717504744928</v>
+        <v>0.005704838249311408</v>
       </c>
     </row>
     <row r="546">
@@ -12985,14 +12985,14 @@
       </c>
       <c r="C546" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Neisseria</t>
         </is>
       </c>
       <c r="D546" t="n">
         <v>0</v>
       </c>
       <c r="E546" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.0003247717504744928</v>
       </c>
     </row>
     <row r="547">
@@ -13031,14 +13031,14 @@
       </c>
       <c r="C548" t="inlineStr">
         <is>
-          <t>Ezakiella</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D548" t="n">
         <v>0</v>
       </c>
       <c r="E548" t="n">
-        <v>0.002980975725860719</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="549">
@@ -13054,14 +13054,14 @@
       </c>
       <c r="C549" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Varibaculum</t>
         </is>
       </c>
       <c r="D549" t="n">
         <v>0</v>
       </c>
       <c r="E549" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.006990870234154651</v>
       </c>
     </row>
     <row r="550">
@@ -13077,14 +13077,14 @@
       </c>
       <c r="C550" t="inlineStr">
         <is>
-          <t>Varibaculum</t>
+          <t>Ezakiella</t>
         </is>
       </c>
       <c r="D550" t="n">
         <v>0</v>
       </c>
       <c r="E550" t="n">
-        <v>0.006990870234154651</v>
+        <v>0.002980975725860719</v>
       </c>
     </row>
     <row r="551">
@@ -13215,14 +13215,14 @@
       </c>
       <c r="C556" t="inlineStr">
         <is>
-          <t>Haemophilus</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D556" t="n">
         <v>0</v>
       </c>
       <c r="E556" t="n">
-        <v>0.005704838249311408</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="557">
@@ -13238,14 +13238,14 @@
       </c>
       <c r="C557" t="inlineStr">
         <is>
-          <t>Neisseria</t>
+          <t>Haemophilus</t>
         </is>
       </c>
       <c r="D557" t="n">
         <v>0</v>
       </c>
       <c r="E557" t="n">
-        <v>0.0003247717504744928</v>
+        <v>0.005704838249311408</v>
       </c>
     </row>
     <row r="558">
@@ -13261,14 +13261,14 @@
       </c>
       <c r="C558" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Neisseria</t>
         </is>
       </c>
       <c r="D558" t="n">
         <v>0</v>
       </c>
       <c r="E558" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.0003247717504744928</v>
       </c>
     </row>
     <row r="559">
@@ -13307,14 +13307,14 @@
       </c>
       <c r="C560" t="inlineStr">
         <is>
-          <t>Ezakiella</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D560" t="n">
         <v>0</v>
       </c>
       <c r="E560" t="n">
-        <v>0.002980975725860719</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="561">
@@ -13330,14 +13330,14 @@
       </c>
       <c r="C561" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Varibaculum</t>
         </is>
       </c>
       <c r="D561" t="n">
         <v>0</v>
       </c>
       <c r="E561" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.006990870234154651</v>
       </c>
     </row>
     <row r="562">
@@ -13353,14 +13353,14 @@
       </c>
       <c r="C562" t="inlineStr">
         <is>
-          <t>Varibaculum</t>
+          <t>Ezakiella</t>
         </is>
       </c>
       <c r="D562" t="n">
         <v>0</v>
       </c>
       <c r="E562" t="n">
-        <v>0.006990870234154651</v>
+        <v>0.002980975725860719</v>
       </c>
     </row>
     <row r="563">
@@ -13491,14 +13491,14 @@
       </c>
       <c r="C568" t="inlineStr">
         <is>
-          <t>Haemophilus</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D568" t="n">
         <v>0</v>
       </c>
       <c r="E568" t="n">
-        <v>0.005704838249311408</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="569">
@@ -13514,14 +13514,14 @@
       </c>
       <c r="C569" t="inlineStr">
         <is>
-          <t>Neisseria</t>
+          <t>Haemophilus</t>
         </is>
       </c>
       <c r="D569" t="n">
         <v>0</v>
       </c>
       <c r="E569" t="n">
-        <v>0.0003247717504744928</v>
+        <v>0.005704838249311408</v>
       </c>
     </row>
     <row r="570">
@@ -13537,14 +13537,14 @@
       </c>
       <c r="C570" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Neisseria</t>
         </is>
       </c>
       <c r="D570" t="n">
         <v>0</v>
       </c>
       <c r="E570" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.0003247717504744928</v>
       </c>
     </row>
     <row r="571">
@@ -13583,14 +13583,14 @@
       </c>
       <c r="C572" t="inlineStr">
         <is>
-          <t>Ezakiella</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D572" t="n">
         <v>0</v>
       </c>
       <c r="E572" t="n">
-        <v>0.002980975725860719</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="573">
@@ -13606,14 +13606,14 @@
       </c>
       <c r="C573" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Varibaculum</t>
         </is>
       </c>
       <c r="D573" t="n">
         <v>0</v>
       </c>
       <c r="E573" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.006990870234154651</v>
       </c>
     </row>
     <row r="574">
@@ -13629,14 +13629,14 @@
       </c>
       <c r="C574" t="inlineStr">
         <is>
-          <t>Varibaculum</t>
+          <t>Ezakiella</t>
         </is>
       </c>
       <c r="D574" t="n">
         <v>0</v>
       </c>
       <c r="E574" t="n">
-        <v>0.006990870234154651</v>
+        <v>0.002980975725860719</v>
       </c>
     </row>
     <row r="575">
@@ -13790,14 +13790,14 @@
       </c>
       <c r="C581" t="inlineStr">
         <is>
-          <t>Neisseria</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D581" t="n">
         <v>0</v>
       </c>
       <c r="E581" t="n">
-        <v>0.0003247717504744928</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="582">
@@ -13813,14 +13813,14 @@
       </c>
       <c r="C582" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Neisseria</t>
         </is>
       </c>
       <c r="D582" t="n">
         <v>0</v>
       </c>
       <c r="E582" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.0003247717504744928</v>
       </c>
     </row>
     <row r="583">
@@ -13859,14 +13859,14 @@
       </c>
       <c r="C584" t="inlineStr">
         <is>
-          <t>Ezakiella</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D584" t="n">
         <v>0</v>
       </c>
       <c r="E584" t="n">
-        <v>0.002980975725860719</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="585">
@@ -13882,14 +13882,14 @@
       </c>
       <c r="C585" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Varibaculum</t>
         </is>
       </c>
       <c r="D585" t="n">
         <v>0</v>
       </c>
       <c r="E585" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.006990870234154651</v>
       </c>
     </row>
     <row r="586">
@@ -13905,14 +13905,14 @@
       </c>
       <c r="C586" t="inlineStr">
         <is>
-          <t>Varibaculum</t>
+          <t>Ezakiella</t>
         </is>
       </c>
       <c r="D586" t="n">
         <v>0</v>
       </c>
       <c r="E586" t="n">
-        <v>0.006990870234154651</v>
+        <v>0.002980975725860719</v>
       </c>
     </row>
     <row r="587">
@@ -14043,14 +14043,14 @@
       </c>
       <c r="C592" t="inlineStr">
         <is>
-          <t>Haemophilus</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D592" t="n">
         <v>0</v>
       </c>
       <c r="E592" t="n">
-        <v>0.005704838249311408</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="593">
@@ -14066,14 +14066,14 @@
       </c>
       <c r="C593" t="inlineStr">
         <is>
-          <t>Neisseria</t>
+          <t>Haemophilus</t>
         </is>
       </c>
       <c r="D593" t="n">
         <v>0</v>
       </c>
       <c r="E593" t="n">
-        <v>0.0003247717504744928</v>
+        <v>0.005704838249311408</v>
       </c>
     </row>
     <row r="594">
@@ -14089,14 +14089,14 @@
       </c>
       <c r="C594" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Neisseria</t>
         </is>
       </c>
       <c r="D594" t="n">
         <v>0</v>
       </c>
       <c r="E594" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.0003247717504744928</v>
       </c>
     </row>
     <row r="595">
@@ -14135,14 +14135,14 @@
       </c>
       <c r="C596" t="inlineStr">
         <is>
-          <t>Ezakiella</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D596" t="n">
         <v>0</v>
       </c>
       <c r="E596" t="n">
-        <v>0.002980975725860719</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="597">
@@ -14158,14 +14158,14 @@
       </c>
       <c r="C597" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Varibaculum</t>
         </is>
       </c>
       <c r="D597" t="n">
         <v>0</v>
       </c>
       <c r="E597" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.006990870234154651</v>
       </c>
     </row>
     <row r="598">
@@ -14181,14 +14181,14 @@
       </c>
       <c r="C598" t="inlineStr">
         <is>
-          <t>Varibaculum</t>
+          <t>Ezakiella</t>
         </is>
       </c>
       <c r="D598" t="n">
         <v>0</v>
       </c>
       <c r="E598" t="n">
-        <v>0.006990870234154651</v>
+        <v>0.002980975725860719</v>
       </c>
     </row>
     <row r="599">
@@ -14319,14 +14319,14 @@
       </c>
       <c r="C604" t="inlineStr">
         <is>
-          <t>Haemophilus</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D604" t="n">
         <v>0</v>
       </c>
       <c r="E604" t="n">
-        <v>0.005704838249311408</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="605">
@@ -14342,14 +14342,14 @@
       </c>
       <c r="C605" t="inlineStr">
         <is>
-          <t>Neisseria</t>
+          <t>Haemophilus</t>
         </is>
       </c>
       <c r="D605" t="n">
         <v>0</v>
       </c>
       <c r="E605" t="n">
-        <v>0.0003247717504744928</v>
+        <v>0.005704838249311408</v>
       </c>
     </row>
     <row r="606">
@@ -14365,14 +14365,14 @@
       </c>
       <c r="C606" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Neisseria</t>
         </is>
       </c>
       <c r="D606" t="n">
         <v>0</v>
       </c>
       <c r="E606" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.0003247717504744928</v>
       </c>
     </row>
     <row r="607">
@@ -14411,14 +14411,14 @@
       </c>
       <c r="C608" t="inlineStr">
         <is>
-          <t>Ezakiella</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D608" t="n">
         <v>0</v>
       </c>
       <c r="E608" t="n">
-        <v>0.002980975725860719</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="609">
@@ -14434,14 +14434,14 @@
       </c>
       <c r="C609" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Varibaculum</t>
         </is>
       </c>
       <c r="D609" t="n">
         <v>0</v>
       </c>
       <c r="E609" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.006990870234154651</v>
       </c>
     </row>
     <row r="610">
@@ -14457,14 +14457,14 @@
       </c>
       <c r="C610" t="inlineStr">
         <is>
-          <t>Varibaculum</t>
+          <t>Ezakiella</t>
         </is>
       </c>
       <c r="D610" t="n">
         <v>0</v>
       </c>
       <c r="E610" t="n">
-        <v>0.006990870234154651</v>
+        <v>0.002980975725860719</v>
       </c>
     </row>
     <row r="611">
@@ -14871,14 +14871,14 @@
       </c>
       <c r="C628" t="inlineStr">
         <is>
-          <t>Haemophilus</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D628" t="n">
         <v>0</v>
       </c>
       <c r="E628" t="n">
-        <v>0.005704838249311408</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="629">
@@ -14894,14 +14894,14 @@
       </c>
       <c r="C629" t="inlineStr">
         <is>
-          <t>Neisseria</t>
+          <t>Haemophilus</t>
         </is>
       </c>
       <c r="D629" t="n">
         <v>0</v>
       </c>
       <c r="E629" t="n">
-        <v>0.0003247717504744928</v>
+        <v>0.005704838249311408</v>
       </c>
     </row>
     <row r="630">
@@ -14917,14 +14917,14 @@
       </c>
       <c r="C630" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Neisseria</t>
         </is>
       </c>
       <c r="D630" t="n">
         <v>0</v>
       </c>
       <c r="E630" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.0003247717504744928</v>
       </c>
     </row>
     <row r="631">
@@ -14963,14 +14963,14 @@
       </c>
       <c r="C632" t="inlineStr">
         <is>
-          <t>Ezakiella</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D632" t="n">
         <v>0</v>
       </c>
       <c r="E632" t="n">
-        <v>0.002980975725860719</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="633">
@@ -14986,14 +14986,14 @@
       </c>
       <c r="C633" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Varibaculum</t>
         </is>
       </c>
       <c r="D633" t="n">
         <v>0</v>
       </c>
       <c r="E633" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.006990870234154651</v>
       </c>
     </row>
     <row r="634">
@@ -15009,14 +15009,14 @@
       </c>
       <c r="C634" t="inlineStr">
         <is>
-          <t>Varibaculum</t>
+          <t>Ezakiella</t>
         </is>
       </c>
       <c r="D634" t="n">
         <v>0</v>
       </c>
       <c r="E634" t="n">
-        <v>0.006990870234154651</v>
+        <v>0.002980975725860719</v>
       </c>
     </row>
     <row r="635">
@@ -15262,14 +15262,14 @@
       </c>
       <c r="C645" t="inlineStr">
         <is>
-          <t>Ezakiella</t>
+          <t>Varibaculum</t>
         </is>
       </c>
       <c r="D645" t="n">
         <v>0</v>
       </c>
       <c r="E645" t="n">
-        <v>0.002980975725860719</v>
+        <v>0.006990870234154651</v>
       </c>
     </row>
     <row r="646">
@@ -15285,14 +15285,14 @@
       </c>
       <c r="C646" t="inlineStr">
         <is>
-          <t>Varibaculum</t>
+          <t>Ezakiella</t>
         </is>
       </c>
       <c r="D646" t="n">
         <v>0</v>
       </c>
       <c r="E646" t="n">
-        <v>0.006990870234154651</v>
+        <v>0.002980975725860719</v>
       </c>
     </row>
     <row r="647">
@@ -15423,14 +15423,14 @@
       </c>
       <c r="C652" t="inlineStr">
         <is>
-          <t>Haemophilus</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D652" t="n">
         <v>0</v>
       </c>
       <c r="E652" t="n">
-        <v>0.005704838249311408</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="653">
@@ -15446,14 +15446,14 @@
       </c>
       <c r="C653" t="inlineStr">
         <is>
-          <t>Neisseria</t>
+          <t>Haemophilus</t>
         </is>
       </c>
       <c r="D653" t="n">
         <v>0</v>
       </c>
       <c r="E653" t="n">
-        <v>0.0003247717504744928</v>
+        <v>0.005704838249311408</v>
       </c>
     </row>
     <row r="654">
@@ -15469,14 +15469,14 @@
       </c>
       <c r="C654" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Neisseria</t>
         </is>
       </c>
       <c r="D654" t="n">
         <v>0</v>
       </c>
       <c r="E654" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.0003247717504744928</v>
       </c>
     </row>
     <row r="655">
@@ -15515,14 +15515,14 @@
       </c>
       <c r="C656" t="inlineStr">
         <is>
-          <t>Ezakiella</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D656" t="n">
         <v>0</v>
       </c>
       <c r="E656" t="n">
-        <v>0.002980975725860719</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="657">
@@ -15538,14 +15538,14 @@
       </c>
       <c r="C657" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Varibaculum</t>
         </is>
       </c>
       <c r="D657" t="n">
         <v>0</v>
       </c>
       <c r="E657" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.006990870234154651</v>
       </c>
     </row>
     <row r="658">
@@ -15561,14 +15561,14 @@
       </c>
       <c r="C658" t="inlineStr">
         <is>
-          <t>Varibaculum</t>
+          <t>Ezakiella</t>
         </is>
       </c>
       <c r="D658" t="n">
         <v>0</v>
       </c>
       <c r="E658" t="n">
-        <v>0.006990870234154651</v>
+        <v>0.002980975725860719</v>
       </c>
     </row>
     <row r="659">
@@ -15722,14 +15722,14 @@
       </c>
       <c r="C665" t="inlineStr">
         <is>
-          <t>Neisseria</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D665" t="n">
         <v>0</v>
       </c>
       <c r="E665" t="n">
-        <v>0.0003247717504744928</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="666">
@@ -15745,14 +15745,14 @@
       </c>
       <c r="C666" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Neisseria</t>
         </is>
       </c>
       <c r="D666" t="n">
         <v>0</v>
       </c>
       <c r="E666" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.0003247717504744928</v>
       </c>
     </row>
     <row r="667">
@@ -15814,14 +15814,14 @@
       </c>
       <c r="C669" t="inlineStr">
         <is>
-          <t>Ezakiella</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D669" t="n">
         <v>0</v>
       </c>
       <c r="E669" t="n">
-        <v>0.002980975725860719</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="670">
@@ -15837,14 +15837,14 @@
       </c>
       <c r="C670" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Ezakiella</t>
         </is>
       </c>
       <c r="D670" t="n">
         <v>0</v>
       </c>
       <c r="E670" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.002980975725860719</v>
       </c>
     </row>
     <row r="671">
@@ -16642,14 +16642,14 @@
       </c>
       <c r="C705" t="inlineStr">
         <is>
-          <t>Ezakiella</t>
+          <t>Varibaculum</t>
         </is>
       </c>
       <c r="D705" t="n">
         <v>0</v>
       </c>
       <c r="E705" t="n">
-        <v>0.002980975725860719</v>
+        <v>0.006990870234154651</v>
       </c>
     </row>
     <row r="706">
@@ -16665,14 +16665,14 @@
       </c>
       <c r="C706" t="inlineStr">
         <is>
-          <t>Varibaculum</t>
+          <t>Ezakiella</t>
         </is>
       </c>
       <c r="D706" t="n">
         <v>0</v>
       </c>
       <c r="E706" t="n">
-        <v>0.006990870234154651</v>
+        <v>0.002980975725860719</v>
       </c>
     </row>
     <row r="707">
@@ -16803,14 +16803,14 @@
       </c>
       <c r="C712" t="inlineStr">
         <is>
-          <t>Haemophilus</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D712" t="n">
         <v>0</v>
       </c>
       <c r="E712" t="n">
-        <v>0.005704838249311408</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="713">
@@ -16826,14 +16826,14 @@
       </c>
       <c r="C713" t="inlineStr">
         <is>
-          <t>Neisseria</t>
+          <t>Haemophilus</t>
         </is>
       </c>
       <c r="D713" t="n">
         <v>0</v>
       </c>
       <c r="E713" t="n">
-        <v>0.0003247717504744928</v>
+        <v>0.005704838249311408</v>
       </c>
     </row>
     <row r="714">
@@ -16849,14 +16849,14 @@
       </c>
       <c r="C714" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Neisseria</t>
         </is>
       </c>
       <c r="D714" t="n">
         <v>0</v>
       </c>
       <c r="E714" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.0003247717504744928</v>
       </c>
     </row>
     <row r="715">
@@ -16918,14 +16918,14 @@
       </c>
       <c r="C717" t="inlineStr">
         <is>
-          <t>Ezakiella</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D717" t="n">
         <v>0</v>
       </c>
       <c r="E717" t="n">
-        <v>0.002980975725860719</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="718">
@@ -16941,14 +16941,14 @@
       </c>
       <c r="C718" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Ezakiella</t>
         </is>
       </c>
       <c r="D718" t="n">
         <v>0</v>
       </c>
       <c r="E718" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.002980975725860719</v>
       </c>
     </row>
     <row r="719">
@@ -17378,14 +17378,14 @@
       </c>
       <c r="C737" t="inlineStr">
         <is>
-          <t>Neisseria</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D737" t="n">
         <v>0</v>
       </c>
       <c r="E737" t="n">
-        <v>0.0003247717504744928</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="738">
@@ -17401,14 +17401,14 @@
       </c>
       <c r="C738" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Neisseria</t>
         </is>
       </c>
       <c r="D738" t="n">
         <v>0</v>
       </c>
       <c r="E738" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.0003247717504744928</v>
       </c>
     </row>
     <row r="739">
@@ -17447,14 +17447,14 @@
       </c>
       <c r="C740" t="inlineStr">
         <is>
-          <t>Ezakiella</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D740" t="n">
         <v>0</v>
       </c>
       <c r="E740" t="n">
-        <v>0.002980975725860719</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="741">
@@ -17470,14 +17470,14 @@
       </c>
       <c r="C741" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Varibaculum</t>
         </is>
       </c>
       <c r="D741" t="n">
         <v>0</v>
       </c>
       <c r="E741" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.006990870234154651</v>
       </c>
     </row>
     <row r="742">
@@ -17493,14 +17493,14 @@
       </c>
       <c r="C742" t="inlineStr">
         <is>
-          <t>Varibaculum</t>
+          <t>Ezakiella</t>
         </is>
       </c>
       <c r="D742" t="n">
         <v>0</v>
       </c>
       <c r="E742" t="n">
-        <v>0.006990870234154651</v>
+        <v>0.002980975725860719</v>
       </c>
     </row>
     <row r="743">
@@ -17631,14 +17631,14 @@
       </c>
       <c r="C748" t="inlineStr">
         <is>
-          <t>Haemophilus</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D748" t="n">
         <v>0</v>
       </c>
       <c r="E748" t="n">
-        <v>0.005704838249311408</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="749">
@@ -17654,14 +17654,14 @@
       </c>
       <c r="C749" t="inlineStr">
         <is>
-          <t>Neisseria</t>
+          <t>Haemophilus</t>
         </is>
       </c>
       <c r="D749" t="n">
         <v>0</v>
       </c>
       <c r="E749" t="n">
-        <v>0.0003247717504744928</v>
+        <v>0.005704838249311408</v>
       </c>
     </row>
     <row r="750">
@@ -17677,14 +17677,14 @@
       </c>
       <c r="C750" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Neisseria</t>
         </is>
       </c>
       <c r="D750" t="n">
         <v>0</v>
       </c>
       <c r="E750" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.0003247717504744928</v>
       </c>
     </row>
     <row r="751">
@@ -17723,14 +17723,14 @@
       </c>
       <c r="C752" t="inlineStr">
         <is>
-          <t>Ezakiella</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D752" t="n">
         <v>0</v>
       </c>
       <c r="E752" t="n">
-        <v>0.002980975725860719</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="753">
@@ -17746,14 +17746,14 @@
       </c>
       <c r="C753" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Varibaculum</t>
         </is>
       </c>
       <c r="D753" t="n">
         <v>0</v>
       </c>
       <c r="E753" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.006990870234154651</v>
       </c>
     </row>
     <row r="754">
@@ -17769,14 +17769,14 @@
       </c>
       <c r="C754" t="inlineStr">
         <is>
-          <t>Varibaculum</t>
+          <t>Ezakiella</t>
         </is>
       </c>
       <c r="D754" t="n">
         <v>0</v>
       </c>
       <c r="E754" t="n">
-        <v>0.006990870234154651</v>
+        <v>0.002980975725860719</v>
       </c>
     </row>
     <row r="755">
@@ -17907,14 +17907,14 @@
       </c>
       <c r="C760" t="inlineStr">
         <is>
-          <t>Haemophilus</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D760" t="n">
         <v>0</v>
       </c>
       <c r="E760" t="n">
-        <v>0.005704838249311408</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="761">
@@ -17930,14 +17930,14 @@
       </c>
       <c r="C761" t="inlineStr">
         <is>
-          <t>Neisseria</t>
+          <t>Haemophilus</t>
         </is>
       </c>
       <c r="D761" t="n">
         <v>0</v>
       </c>
       <c r="E761" t="n">
-        <v>0.0003247717504744928</v>
+        <v>0.005704838249311408</v>
       </c>
     </row>
     <row r="762">
@@ -17953,14 +17953,14 @@
       </c>
       <c r="C762" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Neisseria</t>
         </is>
       </c>
       <c r="D762" t="n">
         <v>0</v>
       </c>
       <c r="E762" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.0003247717504744928</v>
       </c>
     </row>
     <row r="763">
@@ -17999,14 +17999,14 @@
       </c>
       <c r="C764" t="inlineStr">
         <is>
-          <t>Ezakiella</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D764" t="n">
         <v>0</v>
       </c>
       <c r="E764" t="n">
-        <v>0.002980975725860719</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="765">
@@ -18022,14 +18022,14 @@
       </c>
       <c r="C765" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Varibaculum</t>
         </is>
       </c>
       <c r="D765" t="n">
         <v>0</v>
       </c>
       <c r="E765" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.006990870234154651</v>
       </c>
     </row>
     <row r="766">
@@ -18045,14 +18045,14 @@
       </c>
       <c r="C766" t="inlineStr">
         <is>
-          <t>Varibaculum</t>
+          <t>Ezakiella</t>
         </is>
       </c>
       <c r="D766" t="n">
         <v>0</v>
       </c>
       <c r="E766" t="n">
-        <v>0.006990870234154651</v>
+        <v>0.002980975725860719</v>
       </c>
     </row>
     <row r="767">
@@ -18574,14 +18574,14 @@
       </c>
       <c r="C789" t="inlineStr">
         <is>
-          <t>Ezakiella</t>
+          <t>Varibaculum</t>
         </is>
       </c>
       <c r="D789" t="n">
         <v>0</v>
       </c>
       <c r="E789" t="n">
-        <v>0.002980975725860719</v>
+        <v>0.006990870234154651</v>
       </c>
     </row>
     <row r="790">
@@ -18597,14 +18597,14 @@
       </c>
       <c r="C790" t="inlineStr">
         <is>
-          <t>Varibaculum</t>
+          <t>Ezakiella</t>
         </is>
       </c>
       <c r="D790" t="n">
         <v>0</v>
       </c>
       <c r="E790" t="n">
-        <v>0.006990870234154651</v>
+        <v>0.002980975725860719</v>
       </c>
     </row>
     <row r="791">
@@ -19011,14 +19011,14 @@
       </c>
       <c r="C808" t="inlineStr">
         <is>
-          <t>Haemophilus</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D808" t="n">
         <v>0</v>
       </c>
       <c r="E808" t="n">
-        <v>0.005704838249311408</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="809">
@@ -19034,14 +19034,14 @@
       </c>
       <c r="C809" t="inlineStr">
         <is>
-          <t>Neisseria</t>
+          <t>Haemophilus</t>
         </is>
       </c>
       <c r="D809" t="n">
         <v>0</v>
       </c>
       <c r="E809" t="n">
-        <v>0.0003247717504744928</v>
+        <v>0.005704838249311408</v>
       </c>
     </row>
     <row r="810">
@@ -19057,14 +19057,14 @@
       </c>
       <c r="C810" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Neisseria</t>
         </is>
       </c>
       <c r="D810" t="n">
         <v>0</v>
       </c>
       <c r="E810" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.0003247717504744928</v>
       </c>
     </row>
     <row r="811">
@@ -19103,14 +19103,14 @@
       </c>
       <c r="C812" t="inlineStr">
         <is>
-          <t>Ezakiella</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D812" t="n">
         <v>0</v>
       </c>
       <c r="E812" t="n">
-        <v>0.002980975725860719</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="813">
@@ -19126,14 +19126,14 @@
       </c>
       <c r="C813" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Varibaculum</t>
         </is>
       </c>
       <c r="D813" t="n">
         <v>0</v>
       </c>
       <c r="E813" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.006990870234154651</v>
       </c>
     </row>
     <row r="814">
@@ -19149,14 +19149,14 @@
       </c>
       <c r="C814" t="inlineStr">
         <is>
-          <t>Varibaculum</t>
+          <t>Ezakiella</t>
         </is>
       </c>
       <c r="D814" t="n">
         <v>0</v>
       </c>
       <c r="E814" t="n">
-        <v>0.006990870234154651</v>
+        <v>0.002980975725860719</v>
       </c>
     </row>
     <row r="815">
@@ -19310,14 +19310,14 @@
       </c>
       <c r="C821" t="inlineStr">
         <is>
-          <t>Neisseria</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D821" t="n">
         <v>0</v>
       </c>
       <c r="E821" t="n">
-        <v>0.0003247717504744928</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="822">
@@ -19333,14 +19333,14 @@
       </c>
       <c r="C822" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Neisseria</t>
         </is>
       </c>
       <c r="D822" t="n">
         <v>0</v>
       </c>
       <c r="E822" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.0003247717504744928</v>
       </c>
     </row>
     <row r="823">
@@ -19379,14 +19379,14 @@
       </c>
       <c r="C824" t="inlineStr">
         <is>
-          <t>Ezakiella</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D824" t="n">
         <v>0</v>
       </c>
       <c r="E824" t="n">
-        <v>0.002980975725860719</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="825">
@@ -19402,14 +19402,14 @@
       </c>
       <c r="C825" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Varibaculum</t>
         </is>
       </c>
       <c r="D825" t="n">
         <v>0</v>
       </c>
       <c r="E825" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.006990870234154651</v>
       </c>
     </row>
     <row r="826">
@@ -19425,14 +19425,14 @@
       </c>
       <c r="C826" t="inlineStr">
         <is>
-          <t>Varibaculum</t>
+          <t>Ezakiella</t>
         </is>
       </c>
       <c r="D826" t="n">
         <v>0</v>
       </c>
       <c r="E826" t="n">
-        <v>0.006990870234154651</v>
+        <v>0.002980975725860719</v>
       </c>
     </row>
     <row r="827">
@@ -20115,14 +20115,14 @@
       </c>
       <c r="C856" t="inlineStr">
         <is>
-          <t>Haemophilus</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D856" t="n">
         <v>0</v>
       </c>
       <c r="E856" t="n">
-        <v>0.005704838249311408</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="857">
@@ -20138,14 +20138,14 @@
       </c>
       <c r="C857" t="inlineStr">
         <is>
-          <t>Neisseria</t>
+          <t>Haemophilus</t>
         </is>
       </c>
       <c r="D857" t="n">
         <v>0</v>
       </c>
       <c r="E857" t="n">
-        <v>0.0003247717504744928</v>
+        <v>0.005704838249311408</v>
       </c>
     </row>
     <row r="858">
@@ -20161,14 +20161,14 @@
       </c>
       <c r="C858" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Neisseria</t>
         </is>
       </c>
       <c r="D858" t="n">
         <v>0</v>
       </c>
       <c r="E858" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.0003247717504744928</v>
       </c>
     </row>
     <row r="859">
@@ -20207,14 +20207,14 @@
       </c>
       <c r="C860" t="inlineStr">
         <is>
-          <t>Ezakiella</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D860" t="n">
         <v>0</v>
       </c>
       <c r="E860" t="n">
-        <v>0.002980975725860719</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="861">
@@ -20230,14 +20230,14 @@
       </c>
       <c r="C861" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Varibaculum</t>
         </is>
       </c>
       <c r="D861" t="n">
         <v>0</v>
       </c>
       <c r="E861" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.006990870234154651</v>
       </c>
     </row>
     <row r="862">
@@ -20253,14 +20253,14 @@
       </c>
       <c r="C862" t="inlineStr">
         <is>
-          <t>Varibaculum</t>
+          <t>Ezakiella</t>
         </is>
       </c>
       <c r="D862" t="n">
         <v>0</v>
       </c>
       <c r="E862" t="n">
-        <v>0.006990870234154651</v>
+        <v>0.002980975725860719</v>
       </c>
     </row>
     <row r="863">
@@ -20391,14 +20391,14 @@
       </c>
       <c r="C868" t="inlineStr">
         <is>
-          <t>Haemophilus</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D868" t="n">
         <v>0</v>
       </c>
       <c r="E868" t="n">
-        <v>0.005704838249311408</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="869">
@@ -20414,14 +20414,14 @@
       </c>
       <c r="C869" t="inlineStr">
         <is>
-          <t>Neisseria</t>
+          <t>Haemophilus</t>
         </is>
       </c>
       <c r="D869" t="n">
         <v>0</v>
       </c>
       <c r="E869" t="n">
-        <v>0.0003247717504744928</v>
+        <v>0.005704838249311408</v>
       </c>
     </row>
     <row r="870">
@@ -20437,14 +20437,14 @@
       </c>
       <c r="C870" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Neisseria</t>
         </is>
       </c>
       <c r="D870" t="n">
         <v>0</v>
       </c>
       <c r="E870" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.0003247717504744928</v>
       </c>
     </row>
     <row r="871">
@@ -20483,14 +20483,14 @@
       </c>
       <c r="C872" t="inlineStr">
         <is>
-          <t>Ezakiella</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D872" t="n">
         <v>0</v>
       </c>
       <c r="E872" t="n">
-        <v>0.002980975725860719</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="873">
@@ -20506,14 +20506,14 @@
       </c>
       <c r="C873" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Varibaculum</t>
         </is>
       </c>
       <c r="D873" t="n">
         <v>0</v>
       </c>
       <c r="E873" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.006990870234154651</v>
       </c>
     </row>
     <row r="874">
@@ -20529,14 +20529,14 @@
       </c>
       <c r="C874" t="inlineStr">
         <is>
-          <t>Varibaculum</t>
+          <t>Ezakiella</t>
         </is>
       </c>
       <c r="D874" t="n">
         <v>0</v>
       </c>
       <c r="E874" t="n">
-        <v>0.006990870234154651</v>
+        <v>0.002980975725860719</v>
       </c>
     </row>
     <row r="875">
@@ -20782,14 +20782,14 @@
       </c>
       <c r="C885" t="inlineStr">
         <is>
-          <t>Ezakiella</t>
+          <t>Varibaculum</t>
         </is>
       </c>
       <c r="D885" t="n">
         <v>0</v>
       </c>
       <c r="E885" t="n">
-        <v>0.002980975725860719</v>
+        <v>0.006990870234154651</v>
       </c>
     </row>
     <row r="886">
@@ -20805,14 +20805,14 @@
       </c>
       <c r="C886" t="inlineStr">
         <is>
-          <t>Varibaculum</t>
+          <t>Ezakiella</t>
         </is>
       </c>
       <c r="D886" t="n">
         <v>0</v>
       </c>
       <c r="E886" t="n">
-        <v>0.006990870234154651</v>
+        <v>0.002980975725860719</v>
       </c>
     </row>
     <row r="887">
@@ -21219,14 +21219,14 @@
       </c>
       <c r="C904" t="inlineStr">
         <is>
-          <t>Haemophilus</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D904" t="n">
         <v>0</v>
       </c>
       <c r="E904" t="n">
-        <v>0.005704838249311408</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="905">
@@ -21242,14 +21242,14 @@
       </c>
       <c r="C905" t="inlineStr">
         <is>
-          <t>Neisseria</t>
+          <t>Haemophilus</t>
         </is>
       </c>
       <c r="D905" t="n">
         <v>0</v>
       </c>
       <c r="E905" t="n">
-        <v>0.0003247717504744928</v>
+        <v>0.005704838249311408</v>
       </c>
     </row>
     <row r="906">
@@ -21265,14 +21265,14 @@
       </c>
       <c r="C906" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Neisseria</t>
         </is>
       </c>
       <c r="D906" t="n">
         <v>0</v>
       </c>
       <c r="E906" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.0003247717504744928</v>
       </c>
     </row>
     <row r="907">
@@ -21311,14 +21311,14 @@
       </c>
       <c r="C908" t="inlineStr">
         <is>
-          <t>Ezakiella</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D908" t="n">
         <v>0</v>
       </c>
       <c r="E908" t="n">
-        <v>0.002980975725860719</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="909">
@@ -21334,14 +21334,14 @@
       </c>
       <c r="C909" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Varibaculum</t>
         </is>
       </c>
       <c r="D909" t="n">
         <v>0</v>
       </c>
       <c r="E909" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.006990870234154651</v>
       </c>
     </row>
     <row r="910">
@@ -21357,14 +21357,14 @@
       </c>
       <c r="C910" t="inlineStr">
         <is>
-          <t>Varibaculum</t>
+          <t>Ezakiella</t>
         </is>
       </c>
       <c r="D910" t="n">
         <v>0</v>
       </c>
       <c r="E910" t="n">
-        <v>0.006990870234154651</v>
+        <v>0.002980975725860719</v>
       </c>
     </row>
     <row r="911">
@@ -21771,14 +21771,14 @@
       </c>
       <c r="C928" t="inlineStr">
         <is>
-          <t>Haemophilus</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D928" t="n">
         <v>0</v>
       </c>
       <c r="E928" t="n">
-        <v>0.005704838249311408</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="929">
@@ -21794,14 +21794,14 @@
       </c>
       <c r="C929" t="inlineStr">
         <is>
-          <t>Neisseria</t>
+          <t>Haemophilus</t>
         </is>
       </c>
       <c r="D929" t="n">
         <v>0</v>
       </c>
       <c r="E929" t="n">
-        <v>0.0003247717504744928</v>
+        <v>0.005704838249311408</v>
       </c>
     </row>
     <row r="930">
@@ -21817,14 +21817,14 @@
       </c>
       <c r="C930" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Neisseria</t>
         </is>
       </c>
       <c r="D930" t="n">
         <v>0</v>
       </c>
       <c r="E930" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.0003247717504744928</v>
       </c>
     </row>
     <row r="931">
@@ -21863,14 +21863,14 @@
       </c>
       <c r="C932" t="inlineStr">
         <is>
-          <t>Ezakiella</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D932" t="n">
         <v>0</v>
       </c>
       <c r="E932" t="n">
-        <v>0.002980975725860719</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="933">
@@ -21886,14 +21886,14 @@
       </c>
       <c r="C933" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Varibaculum</t>
         </is>
       </c>
       <c r="D933" t="n">
         <v>0</v>
       </c>
       <c r="E933" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.006990870234154651</v>
       </c>
     </row>
     <row r="934">
@@ -21909,14 +21909,14 @@
       </c>
       <c r="C934" t="inlineStr">
         <is>
-          <t>Varibaculum</t>
+          <t>Ezakiella</t>
         </is>
       </c>
       <c r="D934" t="n">
         <v>0</v>
       </c>
       <c r="E934" t="n">
-        <v>0.006990870234154651</v>
+        <v>0.002980975725860719</v>
       </c>
     </row>
     <row r="935">
@@ -22070,14 +22070,14 @@
       </c>
       <c r="C941" t="inlineStr">
         <is>
-          <t>Neisseria</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D941" t="n">
         <v>0</v>
       </c>
       <c r="E941" t="n">
-        <v>0.0003247717504744928</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="942">
@@ -22093,14 +22093,14 @@
       </c>
       <c r="C942" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Neisseria</t>
         </is>
       </c>
       <c r="D942" t="n">
         <v>0</v>
       </c>
       <c r="E942" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.0003247717504744928</v>
       </c>
     </row>
     <row r="943">
@@ -22162,14 +22162,14 @@
       </c>
       <c r="C945" t="inlineStr">
         <is>
-          <t>Ezakiella</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D945" t="n">
         <v>0</v>
       </c>
       <c r="E945" t="n">
-        <v>0.002980975725860719</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="946">
@@ -22185,14 +22185,14 @@
       </c>
       <c r="C946" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Ezakiella</t>
         </is>
       </c>
       <c r="D946" t="n">
         <v>0</v>
       </c>
       <c r="E946" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.002980975725860719</v>
       </c>
     </row>
     <row r="947">
@@ -22599,14 +22599,14 @@
       </c>
       <c r="C964" t="inlineStr">
         <is>
-          <t>Haemophilus</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D964" t="n">
         <v>0</v>
       </c>
       <c r="E964" t="n">
-        <v>0.005704838249311408</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="965">
@@ -22622,14 +22622,14 @@
       </c>
       <c r="C965" t="inlineStr">
         <is>
-          <t>Neisseria</t>
+          <t>Haemophilus</t>
         </is>
       </c>
       <c r="D965" t="n">
         <v>0</v>
       </c>
       <c r="E965" t="n">
-        <v>0.0003247717504744928</v>
+        <v>0.005704838249311408</v>
       </c>
     </row>
     <row r="966">
@@ -22645,14 +22645,14 @@
       </c>
       <c r="C966" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Neisseria</t>
         </is>
       </c>
       <c r="D966" t="n">
         <v>0</v>
       </c>
       <c r="E966" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.0003247717504744928</v>
       </c>
     </row>
     <row r="967">
@@ -22691,14 +22691,14 @@
       </c>
       <c r="C968" t="inlineStr">
         <is>
-          <t>Ezakiella</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D968" t="n">
         <v>0</v>
       </c>
       <c r="E968" t="n">
-        <v>0.002980975725860719</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="969">
@@ -22714,14 +22714,14 @@
       </c>
       <c r="C969" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Varibaculum</t>
         </is>
       </c>
       <c r="D969" t="n">
         <v>0</v>
       </c>
       <c r="E969" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.006990870234154651</v>
       </c>
     </row>
     <row r="970">
@@ -22737,14 +22737,14 @@
       </c>
       <c r="C970" t="inlineStr">
         <is>
-          <t>Varibaculum</t>
+          <t>Ezakiella</t>
         </is>
       </c>
       <c r="D970" t="n">
         <v>0</v>
       </c>
       <c r="E970" t="n">
-        <v>0.006990870234154651</v>
+        <v>0.002980975725860719</v>
       </c>
     </row>
     <row r="971">
@@ -23266,14 +23266,14 @@
       </c>
       <c r="C993" t="inlineStr">
         <is>
-          <t>Ezakiella</t>
+          <t>Varibaculum</t>
         </is>
       </c>
       <c r="D993" t="n">
         <v>0</v>
       </c>
       <c r="E993" t="n">
-        <v>0.002980975725860719</v>
+        <v>0.006990870234154651</v>
       </c>
     </row>
     <row r="994">
@@ -23289,14 +23289,14 @@
       </c>
       <c r="C994" t="inlineStr">
         <is>
-          <t>Varibaculum</t>
+          <t>Ezakiella</t>
         </is>
       </c>
       <c r="D994" t="n">
         <v>0</v>
       </c>
       <c r="E994" t="n">
-        <v>0.006990870234154651</v>
+        <v>0.002980975725860719</v>
       </c>
     </row>
     <row r="995">
@@ -23703,14 +23703,14 @@
       </c>
       <c r="C1012" t="inlineStr">
         <is>
-          <t>Haemophilus</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D1012" t="n">
         <v>0</v>
       </c>
       <c r="E1012" t="n">
-        <v>0.005704838249311408</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="1013">
@@ -23726,14 +23726,14 @@
       </c>
       <c r="C1013" t="inlineStr">
         <is>
-          <t>Neisseria</t>
+          <t>Haemophilus</t>
         </is>
       </c>
       <c r="D1013" t="n">
         <v>0</v>
       </c>
       <c r="E1013" t="n">
-        <v>0.0003247717504744928</v>
+        <v>0.005704838249311408</v>
       </c>
     </row>
     <row r="1014">
@@ -23749,14 +23749,14 @@
       </c>
       <c r="C1014" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Neisseria</t>
         </is>
       </c>
       <c r="D1014" t="n">
         <v>0</v>
       </c>
       <c r="E1014" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.0003247717504744928</v>
       </c>
     </row>
     <row r="1015">
@@ -23818,14 +23818,14 @@
       </c>
       <c r="C1017" t="inlineStr">
         <is>
-          <t>Ezakiella</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D1017" t="n">
         <v>0</v>
       </c>
       <c r="E1017" t="n">
-        <v>0.002980975725860719</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="1018">
@@ -23841,14 +23841,14 @@
       </c>
       <c r="C1018" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Ezakiella</t>
         </is>
       </c>
       <c r="D1018" t="n">
         <v>0</v>
       </c>
       <c r="E1018" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.002980975725860719</v>
       </c>
     </row>
     <row r="1019">
@@ -24094,14 +24094,14 @@
       </c>
       <c r="C1029" t="inlineStr">
         <is>
-          <t>Ezakiella</t>
+          <t>Varibaculum</t>
         </is>
       </c>
       <c r="D1029" t="n">
         <v>0</v>
       </c>
       <c r="E1029" t="n">
-        <v>0.002980975725860719</v>
+        <v>0.006990870234154651</v>
       </c>
     </row>
     <row r="1030">
@@ -24117,14 +24117,14 @@
       </c>
       <c r="C1030" t="inlineStr">
         <is>
-          <t>Varibaculum</t>
+          <t>Ezakiella</t>
         </is>
       </c>
       <c r="D1030" t="n">
         <v>0</v>
       </c>
       <c r="E1030" t="n">
-        <v>0.006990870234154651</v>
+        <v>0.002980975725860719</v>
       </c>
     </row>
     <row r="1031">
@@ -24554,14 +24554,14 @@
       </c>
       <c r="C1049" t="inlineStr">
         <is>
-          <t>Neisseria</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D1049" t="n">
         <v>0</v>
       </c>
       <c r="E1049" t="n">
-        <v>0.0003247717504744928</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="1050">
@@ -24577,14 +24577,14 @@
       </c>
       <c r="C1050" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Neisseria</t>
         </is>
       </c>
       <c r="D1050" t="n">
         <v>0</v>
       </c>
       <c r="E1050" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.0003247717504744928</v>
       </c>
     </row>
     <row r="1051">
@@ -24830,14 +24830,14 @@
       </c>
       <c r="C1061" t="inlineStr">
         <is>
-          <t>Neisseria</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D1061" t="n">
         <v>0</v>
       </c>
       <c r="E1061" t="n">
-        <v>0.0003247717504744928</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="1062">
@@ -24853,14 +24853,14 @@
       </c>
       <c r="C1062" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Neisseria</t>
         </is>
       </c>
       <c r="D1062" t="n">
         <v>0</v>
       </c>
       <c r="E1062" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.0003247717504744928</v>
       </c>
     </row>
     <row r="1063">
@@ -24922,14 +24922,14 @@
       </c>
       <c r="C1065" t="inlineStr">
         <is>
-          <t>Ezakiella</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D1065" t="n">
         <v>0</v>
       </c>
       <c r="E1065" t="n">
-        <v>0.002980975725860719</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="1066">
@@ -24945,14 +24945,14 @@
       </c>
       <c r="C1066" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Ezakiella</t>
         </is>
       </c>
       <c r="D1066" t="n">
         <v>0</v>
       </c>
       <c r="E1066" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.002980975725860719</v>
       </c>
     </row>
     <row r="1067">
@@ -25083,14 +25083,14 @@
       </c>
       <c r="C1072" t="inlineStr">
         <is>
-          <t>Haemophilus</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D1072" t="n">
         <v>0</v>
       </c>
       <c r="E1072" t="n">
-        <v>0.005704838249311408</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="1073">
@@ -25106,14 +25106,14 @@
       </c>
       <c r="C1073" t="inlineStr">
         <is>
-          <t>Neisseria</t>
+          <t>Haemophilus</t>
         </is>
       </c>
       <c r="D1073" t="n">
         <v>0</v>
       </c>
       <c r="E1073" t="n">
-        <v>0.0003247717504744928</v>
+        <v>0.005704838249311408</v>
       </c>
     </row>
     <row r="1074">
@@ -25129,14 +25129,14 @@
       </c>
       <c r="C1074" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Neisseria</t>
         </is>
       </c>
       <c r="D1074" t="n">
         <v>0</v>
       </c>
       <c r="E1074" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.0003247717504744928</v>
       </c>
     </row>
     <row r="1075">
@@ -25175,14 +25175,14 @@
       </c>
       <c r="C1076" t="inlineStr">
         <is>
-          <t>Ezakiella</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D1076" t="n">
         <v>0</v>
       </c>
       <c r="E1076" t="n">
-        <v>0.002980975725860719</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="1077">
@@ -25198,14 +25198,14 @@
       </c>
       <c r="C1077" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Varibaculum</t>
         </is>
       </c>
       <c r="D1077" t="n">
         <v>0</v>
       </c>
       <c r="E1077" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.006990870234154651</v>
       </c>
     </row>
     <row r="1078">
@@ -25221,14 +25221,14 @@
       </c>
       <c r="C1078" t="inlineStr">
         <is>
-          <t>Varibaculum</t>
+          <t>Ezakiella</t>
         </is>
       </c>
       <c r="D1078" t="n">
         <v>0</v>
       </c>
       <c r="E1078" t="n">
-        <v>0.006990870234154651</v>
+        <v>0.002980975725860719</v>
       </c>
     </row>
     <row r="1079">
@@ -25359,14 +25359,14 @@
       </c>
       <c r="C1084" t="inlineStr">
         <is>
-          <t>Haemophilus</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D1084" t="n">
         <v>0</v>
       </c>
       <c r="E1084" t="n">
-        <v>0.005704838249311408</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="1085">
@@ -25382,14 +25382,14 @@
       </c>
       <c r="C1085" t="inlineStr">
         <is>
-          <t>Neisseria</t>
+          <t>Haemophilus</t>
         </is>
       </c>
       <c r="D1085" t="n">
         <v>0</v>
       </c>
       <c r="E1085" t="n">
-        <v>0.0003247717504744928</v>
+        <v>0.005704838249311408</v>
       </c>
     </row>
     <row r="1086">
@@ -25405,14 +25405,14 @@
       </c>
       <c r="C1086" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Neisseria</t>
         </is>
       </c>
       <c r="D1086" t="n">
         <v>0</v>
       </c>
       <c r="E1086" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.0003247717504744928</v>
       </c>
     </row>
     <row r="1087">
@@ -25451,14 +25451,14 @@
       </c>
       <c r="C1088" t="inlineStr">
         <is>
-          <t>Ezakiella</t>
+          <t>Porphyromonas</t>
         </is>
       </c>
       <c r="D1088" t="n">
         <v>0</v>
       </c>
       <c r="E1088" t="n">
-        <v>0.002980975725860719</v>
+        <v>0.00929406095537628</v>
       </c>
     </row>
     <row r="1089">
@@ -25474,14 +25474,14 @@
       </c>
       <c r="C1089" t="inlineStr">
         <is>
-          <t>Porphyromonas</t>
+          <t>Varibaculum</t>
         </is>
       </c>
       <c r="D1089" t="n">
         <v>0</v>
       </c>
       <c r="E1089" t="n">
-        <v>0.00929406095537628</v>
+        <v>0.006990870234154651</v>
       </c>
     </row>
     <row r="1090">
@@ -25497,14 +25497,14 @@
       </c>
       <c r="C1090" t="inlineStr">
         <is>
-          <t>Varibaculum</t>
+          <t>Ezakiella</t>
         </is>
       </c>
       <c r="D1090" t="n">
         <v>0</v>
       </c>
       <c r="E1090" t="n">
-        <v>0.006990870234154651</v>
+        <v>0.002980975725860719</v>
       </c>
     </row>
     <row r="1091">

</xml_diff>